<commit_message>
UPDATE Vistas de Prospectos Editar, Ver, Seeder de tipo jornada y tipo contrato
</commit_message>
<xml_diff>
--- a/EjemploClientes.xlsx
+++ b/EjemploClientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B&amp;W\Documents\DocsPlaneaTuBien\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B&amp;W\Documents\planea\PlaneaTuBien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57C6E6BE-EDAF-4905-B754-B18840554FDA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E619AEF8-A1F8-4DD5-AC18-3F5433F344C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-15" windowWidth="19440" windowHeight="15000" xr2:uid="{119FD499-FD24-4133-9C95-0A739B9A822D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{119FD499-FD24-4133-9C95-0A739B9A822D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Nombre</t>
   </si>
@@ -267,7 +267,13 @@
     <t>mfbanto@gmail.com</t>
   </si>
   <si>
-    <t>clien</t>
+    <t>paniagua</t>
+  </si>
+  <si>
+    <t>Sabines</t>
+  </si>
+  <si>
+    <t>lpaniagua@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -642,7 +648,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,9 +1041,23 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
-      <c r="F20" t="s">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
         <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>5534236787</v>
+      </c>
+      <c r="F20">
+        <v>5543231278</v>
       </c>
     </row>
   </sheetData>
@@ -1060,8 +1080,9 @@
     <hyperlink ref="D10" r:id="rId16" xr:uid="{D979F729-80E4-4419-8265-0A7115932464}"/>
     <hyperlink ref="D8" r:id="rId17" xr:uid="{A93198DB-6C8F-429C-84AB-FE15B58CE6B8}"/>
     <hyperlink ref="D19" r:id="rId18" xr:uid="{C8EF1739-D864-4F4F-A25D-CADC3FB48E81}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{38C79DBD-3EA3-4800-8F92-A7A167A90E5F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>